<commit_message>
making a version of the summary script for 2019
</commit_message>
<xml_diff>
--- a/2019/cleaning_summary/survey_cleaning_compare.xlsx
+++ b/2019/cleaning_summary/survey_cleaning_compare.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SChildress\Documents\GitHub\travel-studies\2019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SChildress\Documents\GitHub\travel-studies\2019\cleaning_summary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D42A46F-3A41-46D8-9B17-897B6A8E1D83}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{829795BE-BAE2-4049-AF6A-BFB677F10516}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-165" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-165" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mode" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,10 @@
     <sheet name="Purpose" sheetId="3" r:id="rId3"/>
     <sheet name="Participation Group" sheetId="4" r:id="rId4"/>
     <sheet name="Household Travelers" sheetId="5" r:id="rId5"/>
-    <sheet name="Trip Lengths" sheetId="6" r:id="rId6"/>
-    <sheet name="Speed" sheetId="7" r:id="rId7"/>
+    <sheet name="Parking Location" sheetId="8" r:id="rId6"/>
+    <sheet name="Trip Lengths" sheetId="6" r:id="rId7"/>
+    <sheet name="Speed" sheetId="7" r:id="rId8"/>
+    <sheet name="Duration" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="72">
   <si>
     <t>Main Mode</t>
   </si>
@@ -168,9 +170,6 @@
     <t>Rulesy</t>
   </si>
   <si>
-    <t>Took a taxi (e.g., Yellow Cab)</t>
-  </si>
-  <si>
     <t>Took a taxi</t>
   </si>
   <si>
@@ -186,16 +185,82 @@
     <t>Notes:</t>
   </si>
   <si>
-    <t xml:space="preserve">The fullly cleaned data has more HOV trips. </t>
+    <t>Total</t>
   </si>
   <si>
-    <t>Total</t>
+    <t>Fewer trips in the cleaned data</t>
+  </si>
+  <si>
+    <t>More HOV trips, less SOV in the cleaned data</t>
+  </si>
+  <si>
+    <t>Fewer transit trips in the cleaned data</t>
+  </si>
+  <si>
+    <t>Notes: Not much change. Something may be wrong with the underlying data here.</t>
+  </si>
+  <si>
+    <t>Auto trip, non-taxi: Park location at end of trip</t>
+  </si>
+  <si>
+    <t>N/A - did not get out of vehicle / was dropped off</t>
+  </si>
+  <si>
+    <t>On the street 2+ blocks from destination</t>
+  </si>
+  <si>
+    <t>On the street by destination</t>
+  </si>
+  <si>
+    <t>Park &amp; Ride lot</t>
+  </si>
+  <si>
+    <t>Parking lot/garage (off-street) 2+ blocks from destination</t>
+  </si>
+  <si>
+    <t>Parking lot/garage (off-street) at destination</t>
+  </si>
+  <si>
+    <t>Personal driveway/garage (e.g. own or friend's/family's)</t>
+  </si>
+  <si>
+    <t>google_duration</t>
+  </si>
+  <si>
+    <t>Rulsey doesn't seem to catch the SOV-HOV shift.</t>
+  </si>
+  <si>
+    <t>Notes: The 2017 uncleaned data has more trips for errands and shopping, and school.  The cleaned data has more trips for the "home" purpose and work and recreation/eat meal.</t>
+  </si>
+  <si>
+    <t>Diff: Cleaned- Uncleaned</t>
+  </si>
+  <si>
+    <t>Diff: Rulesy-Cleaned</t>
+  </si>
+  <si>
+    <t>Notes: Rulesy tended to eliminate more rMove trips than the manual cleaning process.  So it shifted to there being higher share of rSurvey trips over all after Rulesy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes: Cleaning identified the number of travelers where it was missing. </t>
+  </si>
+  <si>
+    <t>Very little change</t>
+  </si>
+  <si>
+    <t>Trip Lengths</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -269,7 +334,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -277,7 +342,6 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -286,6 +350,15 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1881,19 +1954,19 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.25852760736196317</c:v>
+                  <c:v>0.25874240347036082</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.34194274028629862</c:v>
+                  <c:v>0.34173640809478012</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.21094069529652351</c:v>
+                  <c:v>0.21102494321785931</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.3803680981595091E-2</c:v>
+                  <c:v>2.381780606085409E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.16478527607361959</c:v>
+                  <c:v>0.1646784391561458</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2217,6 +2290,320 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Total Trips</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Purpose!$H$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Purpose!$I$24:$K$24</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Uncleaned</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Cleaned</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Rulesy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Purpose!$I$25:$K$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>53817</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51814</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>48871</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E18B-4EA1-B615-0FB45A5C464F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1855672000"/>
+        <c:axId val="1855501136"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1855672000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1855501136"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1855501136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1855672000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3054,6 +3441,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -4566,6 +4993,509 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5113,16 +6043,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1647825</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>933450</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>838200</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5154,14 +6084,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
@@ -5183,6 +6113,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44068FB1-DC57-4B0A-B340-CEED1CB1D423}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5553,10 +6519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R29"/>
+  <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5577,7 +6543,7 @@
         <v>Cleaned</v>
       </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5688,16 +6654,6 @@
         <v>0.21520097939196081</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>50</v>
-      </c>
-    </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
@@ -5705,31 +6661,31 @@
       <c r="F18" t="s">
         <v>36</v>
       </c>
-      <c r="K18" s="6"/>
+      <c r="K18" s="5"/>
       <c r="L18" t="s">
-        <v>47</v>
-      </c>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="6"/>
-      <c r="R18" s="6"/>
-    </row>
-    <row r="19" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
+    </row>
+    <row r="19" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="G19" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="H19" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="I19" s="7" t="s">
+      <c r="I19" s="6" t="s">
         <v>2</v>
       </c>
       <c r="L19"/>
@@ -5742,33 +6698,36 @@
       <c r="O19" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
+      <c r="P19" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
         <v>0</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="5">
         <v>1257</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="8">
         <v>2.3356931824516421E-2</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="6">
         <v>0</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H20" s="6">
+      <c r="H20" s="5">
         <v>1199</v>
       </c>
-      <c r="I20" s="9">
+      <c r="I20" s="8">
         <v>2.3161920951976198E-2</v>
       </c>
-      <c r="J20" s="6">
+      <c r="J20" s="5">
         <f t="shared" ref="J20:J22" si="4">C20-H20</f>
         <v>58</v>
       </c>
@@ -5784,34 +6743,38 @@
       <c r="O20" s="2">
         <v>2.3178943072842281E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
+      <c r="P20" s="5">
+        <f>N20-H20</f>
+        <v>-63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
         <v>1</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="5">
         <v>15204</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="8">
         <v>0.2825129605886616</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="6">
         <v>1</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G21" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H21" s="6">
+      <c r="H21" s="5">
         <v>16509</v>
       </c>
-      <c r="I21" s="9">
+      <c r="I21" s="8">
         <v>0.31891589073909521</v>
       </c>
-      <c r="J21" s="6">
-        <f t="shared" si="4"/>
+      <c r="J21" s="5">
+        <f>C21-H21</f>
         <v>-1305</v>
       </c>
       <c r="L21" s="1">
@@ -5826,33 +6789,37 @@
       <c r="O21" s="2">
         <v>0.28771679249132831</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="7">
+      <c r="P21" s="5">
+        <f t="shared" ref="P21:P25" si="5">N21-H21</f>
+        <v>-2408</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
         <v>2</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="5">
         <v>937</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D22" s="8">
         <v>1.7410855305944221E-2</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="6">
         <v>2</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="G22" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H22" s="6">
+      <c r="H22" s="5">
         <v>909</v>
       </c>
-      <c r="I22" s="9">
+      <c r="I22" s="8">
         <v>1.7559788278020318E-2</v>
       </c>
-      <c r="J22" s="6">
+      <c r="J22" s="5">
         <f t="shared" si="4"/>
         <v>28</v>
       </c>
@@ -5869,36 +6836,39 @@
       <c r="O22" s="2">
         <v>1.7751479289940829E-2</v>
       </c>
-      <c r="P22"/>
+      <c r="P22" s="5">
+        <f t="shared" si="5"/>
+        <v>-39</v>
+      </c>
       <c r="Q22"/>
       <c r="R22"/>
     </row>
-    <row r="23" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="7">
+    <row r="23" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
         <v>3</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="5">
         <v>18206</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="8">
         <v>0.33829459092851699</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="6">
         <v>3</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="G23" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H23" s="6">
+      <c r="H23" s="5">
         <v>16848</v>
       </c>
-      <c r="I23" s="9">
+      <c r="I23" s="8">
         <v>0.32546459065796091</v>
       </c>
-      <c r="J23" s="6">
+      <c r="J23" s="5">
         <f>C23-H23</f>
         <v>1358</v>
       </c>
@@ -5915,37 +6885,40 @@
       <c r="O23" s="2">
         <v>0.33970618241175271</v>
       </c>
-      <c r="P23"/>
+      <c r="P23" s="5">
+        <f t="shared" si="5"/>
+        <v>-199</v>
+      </c>
       <c r="Q23"/>
       <c r="R23"/>
     </row>
-    <row r="24" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="7">
+    <row r="24" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
         <v>4</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="5">
         <v>6123</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D24" s="8">
         <v>0.1137744578850549</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="6">
         <v>4</v>
       </c>
-      <c r="G24" s="6" t="s">
+      <c r="G24" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H24" s="6">
+      <c r="H24" s="5">
         <v>5465</v>
       </c>
-      <c r="I24" s="9">
+      <c r="I24" s="8">
         <v>0.10557122435575469</v>
       </c>
-      <c r="J24" s="6">
-        <f t="shared" ref="J24:J25" si="5">C24-H24</f>
+      <c r="J24" s="5">
+        <f t="shared" ref="J24:J25" si="6">C24-H24</f>
         <v>658</v>
       </c>
       <c r="K24"/>
@@ -5961,37 +6934,40 @@
       <c r="O24" s="2">
         <v>0.11644562334217511</v>
       </c>
-      <c r="P24"/>
+      <c r="P24" s="5">
+        <f t="shared" si="5"/>
+        <v>242</v>
+      </c>
       <c r="Q24"/>
       <c r="R24"/>
     </row>
-    <row r="25" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7">
+    <row r="25" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
         <v>5</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="5">
         <v>12090</v>
       </c>
-      <c r="D25" s="9">
+      <c r="D25" s="8">
         <v>0.22465020346730591</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="6">
         <v>5</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="G25" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H25" s="6">
+      <c r="H25" s="5">
         <v>10836</v>
       </c>
-      <c r="I25" s="9">
+      <c r="I25" s="8">
         <v>0.20932658501719281</v>
       </c>
-      <c r="J25" s="6">
-        <f t="shared" si="5"/>
+      <c r="J25" s="5">
+        <f t="shared" si="6"/>
         <v>1254</v>
       </c>
       <c r="K25"/>
@@ -6007,36 +6983,42 @@
       <c r="O25" s="2">
         <v>0.21520097939196081</v>
       </c>
-      <c r="P25"/>
+      <c r="P25" s="5">
+        <f t="shared" si="5"/>
+        <v>-289</v>
+      </c>
       <c r="Q25"/>
       <c r="R25"/>
     </row>
-    <row r="26" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" s="6">
+    <row r="26" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="5">
         <f>SUM(C20:C25)</f>
         <v>53817</v>
       </c>
-      <c r="H26" s="6">
+      <c r="H26" s="5">
         <f>SUM(H20:H25)</f>
         <v>51766</v>
       </c>
-      <c r="I26" s="10"/>
+      <c r="I26" s="9"/>
       <c r="K26"/>
       <c r="L26"/>
       <c r="M26"/>
-      <c r="N26" s="6">
+      <c r="N26" s="5">
         <f>SUM(N20:N25)</f>
         <v>49010</v>
       </c>
       <c r="O26"/>
-      <c r="P26"/>
+      <c r="P26" s="5">
+        <f>N26-H26</f>
+        <v>-2756</v>
+      </c>
       <c r="Q26"/>
       <c r="R26"/>
     </row>
-    <row r="27" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K27"/>
       <c r="L27"/>
       <c r="M27"/>
@@ -6046,7 +7028,7 @@
       <c r="Q27"/>
       <c r="R27"/>
     </row>
-    <row r="28" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K28"/>
       <c r="L28"/>
       <c r="M28"/>
@@ -6056,7 +7038,10 @@
       <c r="Q28"/>
       <c r="R28"/>
     </row>
-    <row r="29" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="K29"/>
       <c r="L29"/>
       <c r="M29"/>
@@ -6066,6 +7051,30 @@
       <c r="Q29"/>
       <c r="R29"/>
     </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f>C26-H26</f>
+        <v>2051</v>
+      </c>
+      <c r="B30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B31" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6074,10 +7083,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:S34"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6103,7 +7112,7 @@
         <v>Cleaned</v>
       </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6120,7 +7129,7 @@
         <v>2.5187566988210071E-2</v>
       </c>
       <c r="D2" s="2">
-        <f>S28</f>
+        <f>O28</f>
         <v>3.2370675975880669E-2</v>
       </c>
     </row>
@@ -6137,7 +7146,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" ref="D3:D6" si="0">S29</f>
+        <f t="shared" ref="D3:D6" si="0">O29</f>
         <v>8.886067914947636E-3</v>
       </c>
     </row>
@@ -6197,7 +7206,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" s="2">
         <v>0</v>
@@ -6205,7 +7214,7 @@
       <c r="C7" s="2">
         <v>0</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="7">
         <v>0</v>
       </c>
     </row>
@@ -6223,7 +7232,7 @@
         <v>0.91907824222936763</v>
       </c>
       <c r="D8" s="2">
-        <f>S33</f>
+        <f>O33</f>
         <v>0.91526499523960647</v>
       </c>
     </row>
@@ -6259,50 +7268,47 @@
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>35</v>
       </c>
       <c r="F26" t="s">
         <v>36</v>
       </c>
-      <c r="K26" t="s">
-        <v>43</v>
-      </c>
-      <c r="P26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>9</v>
       </c>
@@ -6321,26 +7327,17 @@
       <c r="I27" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L27" s="1" t="s">
+      <c r="M27" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M27" s="1" t="s">
+      <c r="N27" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N27" s="1" t="s">
+      <c r="O27" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q27" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R27" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="S27" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>0</v>
       </c>
@@ -6365,82 +7362,58 @@
       <c r="I28" s="2">
         <v>2.5187566988210071E-2</v>
       </c>
-      <c r="K28" s="1">
+      <c r="L28" s="1">
         <v>0</v>
       </c>
-      <c r="L28" t="s">
+      <c r="M28" t="s">
         <v>10</v>
       </c>
-      <c r="M28">
-        <v>10618</v>
-      </c>
       <c r="N28">
-        <v>0.65778713914013132</v>
-      </c>
-      <c r="P28" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>10</v>
-      </c>
-      <c r="R28">
         <v>102</v>
       </c>
-      <c r="S28" s="2">
+      <c r="O28" s="2">
         <v>3.2370675975880669E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="7">
+    <row r="29" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
         <v>1</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="5">
         <v>5</v>
       </c>
-      <c r="D29" s="11">
+      <c r="D29" s="10">
         <v>2.5562372188139061E-3</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F29" s="6">
         <v>1</v>
       </c>
-      <c r="G29" s="6" t="s">
+      <c r="G29" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H29" s="6">
+      <c r="H29" s="5">
         <v>24</v>
       </c>
-      <c r="I29" s="11">
+      <c r="I29" s="10">
         <v>1.2861736334405139E-2</v>
       </c>
-      <c r="K29" s="7">
+      <c r="L29" s="6">
         <v>1</v>
       </c>
-      <c r="L29" s="6" t="s">
+      <c r="M29" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M29" s="6">
-        <v>3257</v>
-      </c>
-      <c r="N29" s="6">
-        <v>0.201771775492504</v>
-      </c>
-      <c r="P29" s="7">
-        <v>1</v>
-      </c>
-      <c r="Q29" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="R29" s="6">
+      <c r="N29" s="5">
         <v>28</v>
       </c>
-      <c r="S29" s="11">
+      <c r="O29" s="10">
         <v>8.886067914947636E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>2</v>
       </c>
@@ -6465,32 +7438,20 @@
       <c r="I30" s="2">
         <v>2.5723472668810289E-2</v>
       </c>
-      <c r="K30" s="1">
+      <c r="L30" s="1">
         <v>2</v>
       </c>
-      <c r="L30" t="s">
+      <c r="M30" t="s">
         <v>12</v>
       </c>
-      <c r="M30">
-        <v>348</v>
-      </c>
       <c r="N30">
-        <v>2.155866683186718E-2</v>
-      </c>
-      <c r="P30" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>12</v>
-      </c>
-      <c r="R30">
         <v>26</v>
       </c>
-      <c r="S30" s="2">
+      <c r="O30" s="2">
         <v>8.2513487781656625E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>3</v>
       </c>
@@ -6515,32 +7476,20 @@
       <c r="I31" s="2">
         <v>1.7148981779206859E-2</v>
       </c>
-      <c r="K31" s="1">
+      <c r="L31" s="1">
         <v>3</v>
       </c>
-      <c r="L31" t="s">
+      <c r="M31" t="s">
         <v>5</v>
       </c>
-      <c r="M31">
-        <v>32</v>
-      </c>
       <c r="N31">
-        <v>1.982406145459051E-3</v>
-      </c>
-      <c r="P31" s="1">
-        <v>3</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>5</v>
-      </c>
-      <c r="R31">
         <v>46</v>
       </c>
-      <c r="S31" s="2">
+      <c r="O31" s="2">
         <v>1.4598540145985399E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>4</v>
       </c>
@@ -6565,32 +7514,20 @@
       <c r="I32" s="2">
         <v>0.91907824222936763</v>
       </c>
-      <c r="K32" s="1">
+      <c r="L32" s="1">
         <v>4</v>
       </c>
-      <c r="L32" t="s">
+      <c r="M32" t="s">
         <v>13</v>
       </c>
-      <c r="M32">
-        <v>30</v>
-      </c>
       <c r="N32">
-        <v>1.8585057613678599E-3</v>
-      </c>
-      <c r="P32" s="1">
-        <v>4</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>13</v>
-      </c>
-      <c r="R32">
         <v>65</v>
       </c>
-      <c r="S32" s="2">
+      <c r="O32" s="2">
         <v>2.0628371945414149E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>5</v>
       </c>
@@ -6603,43 +7540,22 @@
       <c r="D33" s="2">
         <v>0.90695296523517377</v>
       </c>
-      <c r="K33" s="1">
+      <c r="L33" s="1">
         <v>5</v>
       </c>
-      <c r="L33" t="s">
-        <v>44</v>
-      </c>
-      <c r="M33">
-        <v>47</v>
+      <c r="M33" t="s">
+        <v>14</v>
       </c>
       <c r="N33">
-        <v>2.911659026142981E-3</v>
-      </c>
-      <c r="P33" s="1">
-        <v>5</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>14</v>
-      </c>
-      <c r="R33">
         <v>2884</v>
       </c>
-      <c r="S33" s="2">
+      <c r="O33" s="2">
         <v>0.91526499523960647</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="K34" s="1">
-        <v>6</v>
-      </c>
-      <c r="L34" t="s">
-        <v>14</v>
-      </c>
-      <c r="M34">
-        <v>1810</v>
-      </c>
-      <c r="N34">
-        <v>0.1121298476025276</v>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -6650,156 +7566,156 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:T18"/>
+  <dimension ref="A2:P33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
     <col min="2" max="2" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B2" t="str">
+      <c r="B2" s="14" t="str">
         <f>A12</f>
         <v>Uncleaned</v>
       </c>
-      <c r="C2" t="str">
+      <c r="C2" s="14" t="str">
         <f>F12</f>
         <v>Cleaned</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="16">
         <f>D14</f>
         <v>0.2860434435215638</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="16">
         <f>I14</f>
         <v>0.26031574477940322</v>
       </c>
-      <c r="D3" s="2">
-        <f>O14</f>
-        <v>0.25852760736196317</v>
-      </c>
-      <c r="E3" s="2">
-        <f>T14</f>
+      <c r="D3" s="16">
+        <f>P14</f>
         <v>0.25874240347036082</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="2">
-        <f t="shared" ref="B4:B7" si="0">D15</f>
+      <c r="B4" s="16">
+        <f>D15</f>
         <v>0.30750506345578532</v>
       </c>
-      <c r="C4" s="2">
-        <f t="shared" ref="C4:C7" si="1">I15</f>
+      <c r="C4" s="16">
+        <f>I15</f>
         <v>0.32531748176168601</v>
       </c>
-      <c r="D4" s="2">
-        <f t="shared" ref="D4:D7" si="2">O15</f>
-        <v>0.34194274028629862</v>
-      </c>
-      <c r="E4" s="2">
-        <f t="shared" ref="E4:E7" si="3">T15</f>
+      <c r="D4" s="16">
+        <f t="shared" ref="D4:D7" si="0">P15</f>
         <v>0.34173640809478012</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="16">
+        <f>D16</f>
+        <v>0.21160599810468811</v>
+      </c>
+      <c r="C5" s="16">
+        <f>I16</f>
+        <v>0.2213108426294052</v>
+      </c>
+      <c r="D5" s="16">
         <f t="shared" si="0"/>
-        <v>0.21160599810468811</v>
-      </c>
-      <c r="C5" s="2">
-        <f t="shared" si="1"/>
-        <v>0.2213108426294052</v>
-      </c>
-      <c r="D5" s="2">
-        <f t="shared" si="2"/>
-        <v>0.21094069529652351</v>
-      </c>
-      <c r="E5" s="2">
-        <f t="shared" si="3"/>
         <v>0.21102494321785931</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="16">
+        <f>D17</f>
+        <v>2.8838471115075159E-2</v>
+      </c>
+      <c r="C6" s="16">
+        <f>I17</f>
+        <v>2.2928166132705451E-2</v>
+      </c>
+      <c r="D6" s="16">
         <f t="shared" si="0"/>
-        <v>2.8838471115075159E-2</v>
-      </c>
-      <c r="C6" s="2">
-        <f t="shared" si="1"/>
-        <v>2.2928166132705451E-2</v>
-      </c>
-      <c r="D6" s="2">
-        <f t="shared" si="2"/>
-        <v>2.3803680981595091E-2</v>
-      </c>
-      <c r="E6" s="2">
-        <f t="shared" si="3"/>
         <v>2.381780606085409E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="16">
+        <f>D18</f>
+        <v>0.16600702380288759</v>
+      </c>
+      <c r="C7" s="16">
+        <f>I18</f>
+        <v>0.1701277646968001</v>
+      </c>
+      <c r="D7" s="16">
         <f t="shared" si="0"/>
-        <v>0.16600702380288759</v>
-      </c>
-      <c r="C7" s="2">
-        <f t="shared" si="1"/>
-        <v>0.1701277646968001</v>
-      </c>
-      <c r="D7" s="2">
-        <f t="shared" si="2"/>
-        <v>0.16478527607361959</v>
-      </c>
-      <c r="E7" s="2">
-        <f t="shared" si="3"/>
         <v>0.1646784391561458</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>2017</v>
+      </c>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>35</v>
       </c>
       <c r="F12" t="s">
         <v>36</v>
       </c>
-      <c r="L12" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="M12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>15</v>
       </c>
@@ -6818,26 +7734,17 @@
       <c r="I13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="N13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N13" s="1" t="s">
+      <c r="O13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O13" s="1" t="s">
+      <c r="P13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="R13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="T13" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>0</v>
       </c>
@@ -6866,32 +7773,20 @@
         <f>C14-H14</f>
         <v>1906</v>
       </c>
-      <c r="L14" s="1">
+      <c r="M14" s="1">
         <v>0</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>16</v>
       </c>
-      <c r="N14">
-        <v>12642</v>
-      </c>
       <c r="O14">
-        <v>0.25852760736196317</v>
-      </c>
-      <c r="Q14" s="1">
-        <v>0</v>
-      </c>
-      <c r="R14" t="s">
-        <v>16</v>
-      </c>
-      <c r="S14">
         <v>12645</v>
       </c>
-      <c r="T14">
+      <c r="P14">
         <v>0.25874240347036082</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1</v>
       </c>
@@ -6917,35 +7812,23 @@
         <v>0.32531748176168601</v>
       </c>
       <c r="J15">
-        <f t="shared" ref="J15:J18" si="4">C15-H15</f>
+        <f>C15-H15</f>
         <v>-307</v>
       </c>
-      <c r="L15" s="1">
+      <c r="M15" s="1">
         <v>1</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>17</v>
       </c>
-      <c r="N15">
-        <v>16721</v>
-      </c>
       <c r="O15">
-        <v>0.34194274028629862</v>
-      </c>
-      <c r="Q15" s="1">
-        <v>1</v>
-      </c>
-      <c r="R15" t="s">
-        <v>17</v>
-      </c>
-      <c r="S15">
         <v>16701</v>
       </c>
-      <c r="T15">
+      <c r="P15">
         <v>0.34173640809478012</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>2</v>
       </c>
@@ -6971,35 +7854,23 @@
         <v>0.2213108426294052</v>
       </c>
       <c r="J16">
-        <f t="shared" si="4"/>
+        <f>C16-H16</f>
         <v>-79</v>
       </c>
-      <c r="L16" s="1">
+      <c r="M16" s="1">
         <v>2</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>18</v>
       </c>
-      <c r="N16">
-        <v>10315</v>
-      </c>
       <c r="O16">
-        <v>0.21094069529652351</v>
-      </c>
-      <c r="Q16" s="1">
-        <v>2</v>
-      </c>
-      <c r="R16" t="s">
-        <v>18</v>
-      </c>
-      <c r="S16">
         <v>10313</v>
       </c>
-      <c r="T16">
+      <c r="P16">
         <v>0.21102494321785931</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>3</v>
       </c>
@@ -7025,35 +7896,23 @@
         <v>2.2928166132705451E-2</v>
       </c>
       <c r="J17">
-        <f t="shared" si="4"/>
+        <f>C17-H17</f>
         <v>364</v>
       </c>
-      <c r="L17" s="1">
+      <c r="M17" s="1">
         <v>3</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>19</v>
       </c>
-      <c r="N17">
+      <c r="O17">
         <v>1164</v>
       </c>
-      <c r="O17">
-        <v>2.3803680981595091E-2</v>
-      </c>
-      <c r="Q17" s="1">
-        <v>3</v>
-      </c>
-      <c r="R17" t="s">
-        <v>19</v>
-      </c>
-      <c r="S17">
-        <v>1164</v>
-      </c>
-      <c r="T17">
+      <c r="P17">
         <v>2.381780606085409E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>4</v>
       </c>
@@ -7079,51 +7938,91 @@
         <v>0.1701277646968001</v>
       </c>
       <c r="J18">
-        <f t="shared" si="4"/>
+        <f>C18-H18</f>
         <v>119</v>
       </c>
-      <c r="L18" s="1">
+      <c r="M18" s="1">
         <v>4</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" t="s">
         <v>20</v>
       </c>
-      <c r="N18">
-        <v>8058</v>
-      </c>
       <c r="O18">
-        <v>0.16478527607361959</v>
-      </c>
-      <c r="Q18" s="1">
-        <v>4</v>
-      </c>
-      <c r="R18" t="s">
-        <v>20</v>
-      </c>
-      <c r="S18">
         <v>8048</v>
       </c>
-      <c r="T18">
+      <c r="P18">
         <v>0.1646784391561458</v>
       </c>
     </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <f>SUM(C14:C18)</f>
+        <v>53817</v>
+      </c>
+      <c r="H19">
+        <f>SUM(H14:H18)</f>
+        <v>51814</v>
+      </c>
+      <c r="O19">
+        <f>SUM(O14:O18)</f>
+        <v>48871</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I24" t="s">
+        <v>35</v>
+      </c>
+      <c r="J24" t="s">
+        <v>36</v>
+      </c>
+      <c r="K24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>49</v>
+      </c>
+      <c r="I25">
+        <f>C19</f>
+        <v>53817</v>
+      </c>
+      <c r="J25">
+        <f>H19</f>
+        <v>51814</v>
+      </c>
+      <c r="K25">
+        <f>O19</f>
+        <v>48871</v>
+      </c>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I33">
+        <f>14000-5300</f>
+        <v>8700</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A11:P11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:S9"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>40</v>
       </c>
@@ -7136,13 +8035,10 @@
         <v>Cleaned</v>
       </c>
       <c r="E1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B2" t="str">
         <f>B8</f>
         <v>rMove</v>
@@ -7157,14 +8053,10 @@
       </c>
       <c r="E2" s="2">
         <f>N8</f>
-        <v>0.64966878139572115</v>
-      </c>
-      <c r="F2" s="2">
-        <f>S8</f>
         <v>0.64950435566236109</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B3" t="str">
         <f>B9</f>
         <v>rSurvey</v>
@@ -7179,22 +8071,32 @@
       </c>
       <c r="E3" s="2">
         <f>N9</f>
-        <v>0.35033121860427879</v>
-      </c>
-      <c r="F3" s="2">
-        <f>S9</f>
         <v>0.35049564433763891</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
       <c r="F6" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>65</v>
+      </c>
+      <c r="K6" t="s">
+        <v>43</v>
+      </c>
+      <c r="O6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>21</v>
       </c>
@@ -7222,17 +8124,8 @@
       <c r="N7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>0</v>
       </c>
@@ -7257,6 +8150,10 @@
       <c r="I8">
         <v>0.66722548197820619</v>
       </c>
+      <c r="J8">
+        <f>H8-C8</f>
+        <v>-2272</v>
+      </c>
       <c r="K8" s="1">
         <v>0</v>
       </c>
@@ -7264,25 +8161,17 @@
         <v>22</v>
       </c>
       <c r="M8">
-        <v>32462</v>
+        <v>32433</v>
       </c>
       <c r="N8">
-        <v>0.64966878139572115</v>
-      </c>
-      <c r="P8" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>22</v>
-      </c>
-      <c r="R8">
-        <v>32433</v>
-      </c>
-      <c r="S8">
         <v>0.64950435566236109</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O8">
+        <f>M8-C8</f>
+        <v>-4863</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -7307,6 +8196,10 @@
       <c r="I9">
         <v>0.33277451802179381</v>
       </c>
+      <c r="J9">
+        <f t="shared" ref="J9" si="0">H9-C9</f>
+        <v>-740</v>
+      </c>
       <c r="K9" s="1">
         <v>1</v>
       </c>
@@ -7314,22 +8207,19 @@
         <v>23</v>
       </c>
       <c r="M9">
-        <v>17505</v>
+        <v>17502</v>
       </c>
       <c r="N9">
-        <v>0.35033121860427879</v>
-      </c>
-      <c r="P9" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>23</v>
-      </c>
-      <c r="R9">
-        <v>17502</v>
-      </c>
-      <c r="S9">
         <v>0.35049564433763891</v>
+      </c>
+      <c r="O9">
+        <f t="shared" ref="O9" si="1">M9-C9</f>
+        <v>-706</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -7339,10 +8229,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:T27"/>
+  <dimension ref="A1:T29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="W12" sqref="W12"/>
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7363,7 +8253,7 @@
         <v>43</v>
       </c>
       <c r="E1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -7533,7 +8423,7 @@
         <v>36</v>
       </c>
       <c r="O18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
@@ -7956,6 +8846,11 @@
       </c>
       <c r="D27">
         <v>7.5670221965984429E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -7965,436 +8860,373 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:K24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA8E80E4-964A-4DBF-97B5-B1CEF5AB587F}">
+  <dimension ref="A2:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="B3" sqref="B3:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
+    <col min="7" max="7" width="28.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" s="5" t="str">
-        <f>A15</f>
-        <v>Uncleaned</v>
-      </c>
-      <c r="D1" s="5" t="str">
-        <f>D15</f>
-        <v>Cleaned</v>
-      </c>
-      <c r="E1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="3">
-        <f>B17</f>
-        <v>55496</v>
-      </c>
-      <c r="D2" s="3">
-        <f>E17</f>
-        <v>52485</v>
-      </c>
-      <c r="E2" s="3">
-        <f>H17</f>
-        <v>49959</v>
-      </c>
-      <c r="F2">
-        <f>K17</f>
-        <v>49927</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="3">
-        <f t="shared" ref="C3:C9" si="0">B18</f>
-        <v>10532.358433133521</v>
-      </c>
-      <c r="D3" s="3">
-        <f t="shared" ref="D3:D9" si="1">E18</f>
-        <v>9.6812804408460416</v>
-      </c>
-      <c r="E3" s="3">
-        <f t="shared" ref="E3:E9" si="2">H18</f>
-        <v>10.20647675140259</v>
-      </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F9" si="3">K18</f>
-        <v>10.20172775501298</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="17">
+        <f>D19</f>
+        <v>8.5151323134485979E-2</v>
+      </c>
+      <c r="C3" s="17">
+        <f>I19</f>
+        <v>8.5462924172601595E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="17">
+        <f t="shared" ref="B4:B10" si="0">D20</f>
+        <v>3.6510666545970251E-3</v>
+      </c>
+      <c r="C4" s="17">
+        <f t="shared" ref="C4:C10" si="1">I20</f>
+        <v>3.680651146088934E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="17">
         <f t="shared" si="0"/>
-        <v>130174.7515586768</v>
-      </c>
-      <c r="D4" s="3">
+        <v>0.16106937026643731</v>
+      </c>
+      <c r="C5" s="17">
         <f t="shared" si="1"/>
-        <v>94.892898436960735</v>
-      </c>
-      <c r="E4" s="3">
-        <f t="shared" si="2"/>
-        <v>100.7399308252031</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="3"/>
-        <v>100.7710073442213</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="3">
+        <v>0.16197857442097069</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="17">
         <f t="shared" si="0"/>
+        <v>3.8622853866811498E-3</v>
+      </c>
+      <c r="C6" s="17">
+        <f t="shared" si="1"/>
+        <v>3.9798910766652706E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="17">
+        <f t="shared" si="0"/>
+        <v>1.5690534383392171E-3</v>
+      </c>
+      <c r="C7" s="17">
+        <f t="shared" si="1"/>
+        <v>1.675743611227482E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="17">
+        <f t="shared" si="0"/>
+        <v>5.7632539754382791E-3</v>
+      </c>
+      <c r="C8" s="17">
+        <f t="shared" si="1"/>
+        <v>5.7753306601232872E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="17">
+        <f t="shared" si="0"/>
+        <v>0.49373887329893479</v>
+      </c>
+      <c r="C9" s="17">
+        <f t="shared" si="1"/>
+        <v>0.49218983781195758</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="17">
+        <f t="shared" si="0"/>
+        <v>0.24519477384508609</v>
+      </c>
+      <c r="C10" s="17">
+        <f t="shared" si="1"/>
+        <v>0.24525704710036511</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
         <v>0</v>
       </c>
-      <c r="D5" s="3">
-        <f t="shared" si="1"/>
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19">
+        <v>2822</v>
+      </c>
+      <c r="D19" s="2">
+        <v>8.5151323134485979E-2</v>
+      </c>
+      <c r="F19" s="1">
         <v>0</v>
       </c>
-      <c r="E5" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="3">
-        <f t="shared" si="0"/>
-        <v>6.5565514492500014</v>
-      </c>
-      <c r="D6" s="3">
-        <f t="shared" si="1"/>
-        <v>0.86619144197884357</v>
-      </c>
-      <c r="E6" s="3">
-        <f t="shared" si="2"/>
-        <v>0.86619117400000001</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="3"/>
-        <v>0.86494869959436882</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="3">
-        <f t="shared" si="0"/>
-        <v>1363</v>
-      </c>
-      <c r="D7" s="3">
-        <f t="shared" si="1"/>
-        <v>2.3991141732283459</v>
-      </c>
-      <c r="E7" s="3">
-        <f t="shared" si="2"/>
-        <v>2.419619422572179</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="3"/>
-        <v>2.4171331899999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="3">
-        <f t="shared" si="0"/>
-        <v>5668</v>
-      </c>
-      <c r="D8" s="3">
-        <f t="shared" si="1"/>
-        <v>6.088816312733635</v>
-      </c>
-      <c r="E8" s="3">
-        <f t="shared" si="2"/>
-        <v>6.2068768392587286</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="3"/>
-        <v>6.1963116119999997</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="3">
-        <f t="shared" si="0"/>
-        <v>10713002</v>
-      </c>
-      <c r="D9" s="3">
-        <f t="shared" si="1"/>
-        <v>6656.7508251809431</v>
-      </c>
-      <c r="E9" s="3">
-        <f t="shared" si="2"/>
-        <v>6656.7508251809431</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="3"/>
-        <v>6656.7508251809431</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" t="s">
-        <v>36</v>
-      </c>
-      <c r="G15" t="s">
-        <v>43</v>
-      </c>
-      <c r="J15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17">
-        <v>55496</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17">
-        <v>52485</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H17">
-        <v>49959</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K17">
-        <v>49927</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18">
-        <v>10532.358433133521</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18">
-        <v>9.6812804408460416</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H18">
-        <v>10.20647675140259</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K18">
-        <v>10.20172775501298</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19">
-        <v>130174.7515586768</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19">
-        <v>94.892898436960735</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>28</v>
+      <c r="G19" t="s">
+        <v>55</v>
       </c>
       <c r="H19">
-        <v>100.7399308252031</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K19">
-        <v>100.7710073442213</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>29</v>
+        <v>2856</v>
+      </c>
+      <c r="I19" s="2">
+        <v>8.5462924172601595E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20">
+        <v>121</v>
+      </c>
+      <c r="D20" s="2">
+        <v>3.6510666545970251E-3</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>56</v>
       </c>
       <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21">
-        <v>6.5565514492500014</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E21">
-        <v>0.86619144197884357</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>30</v>
+        <v>123</v>
+      </c>
+      <c r="I20" s="2">
+        <v>3.680651146088934E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21">
+        <v>5338</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.16106937026643731</v>
+      </c>
+      <c r="F21" s="1">
+        <v>2</v>
+      </c>
+      <c r="G21" t="s">
+        <v>57</v>
       </c>
       <c r="H21">
-        <v>0.86619117400000001</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K21">
-        <v>0.86494869959436882</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22">
-        <v>1363</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22">
-        <v>2.3991141732283459</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>31</v>
+        <v>5413</v>
+      </c>
+      <c r="I21" s="2">
+        <v>0.16197857442097069</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>128</v>
+      </c>
+      <c r="D22" s="2">
+        <v>3.8622853866811498E-3</v>
+      </c>
+      <c r="F22" s="1">
+        <v>3</v>
+      </c>
+      <c r="G22" t="s">
+        <v>5</v>
       </c>
       <c r="H22">
-        <v>2.419619422572179</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K22">
-        <v>2.4171331899999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23">
-        <v>5668</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E23">
-        <v>6.088816312733635</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>32</v>
+        <v>133</v>
+      </c>
+      <c r="I22" s="2">
+        <v>3.9798910766652706E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23">
+        <v>52</v>
+      </c>
+      <c r="D23" s="2">
+        <v>1.5690534383392171E-3</v>
+      </c>
+      <c r="F23" s="1">
+        <v>4</v>
+      </c>
+      <c r="G23" t="s">
+        <v>58</v>
       </c>
       <c r="H23">
-        <v>6.2068768392587286</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K23">
-        <v>6.1963116119999997</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24">
-        <v>10713002</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24">
-        <v>6656.7508251809431</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>33</v>
+        <v>56</v>
+      </c>
+      <c r="I23" s="2">
+        <v>1.675743611227482E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24">
+        <v>191</v>
+      </c>
+      <c r="D24" s="2">
+        <v>5.7632539754382791E-3</v>
+      </c>
+      <c r="F24" s="1">
+        <v>5</v>
+      </c>
+      <c r="G24" t="s">
+        <v>59</v>
       </c>
       <c r="H24">
-        <v>6656.7508251809431</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K24">
-        <v>6656.7508251809431</v>
+        <v>193</v>
+      </c>
+      <c r="I24" s="2">
+        <v>5.7753306601232872E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25">
+        <v>16363</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.49373887329893479</v>
+      </c>
+      <c r="F25" s="1">
+        <v>6</v>
+      </c>
+      <c r="G25" t="s">
+        <v>60</v>
+      </c>
+      <c r="H25">
+        <v>16448</v>
+      </c>
+      <c r="I25" s="2">
+        <v>0.49218983781195758</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>7</v>
+      </c>
+      <c r="B26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26">
+        <v>8126</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.24519477384508609</v>
+      </c>
+      <c r="F26" s="1">
+        <v>7</v>
+      </c>
+      <c r="G26" t="s">
+        <v>61</v>
+      </c>
+      <c r="H26">
+        <v>8196</v>
+      </c>
+      <c r="I26" s="2">
+        <v>0.24525704710036511</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -8403,16 +9235,375 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:K22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="L29" sqref="L29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="15" t="str">
+        <f>A16</f>
+        <v>Uncleaned</v>
+      </c>
+      <c r="D2" s="15" t="str">
+        <f>D16</f>
+        <v>Cleaned</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="13">
+        <f>B18</f>
+        <v>55496</v>
+      </c>
+      <c r="D3" s="13">
+        <f>E18</f>
+        <v>52485</v>
+      </c>
+      <c r="E3" s="13">
+        <f>H18</f>
+        <v>49927</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="13">
+        <f t="shared" ref="C4:C10" si="0">B19</f>
+        <v>10532.358433133521</v>
+      </c>
+      <c r="D4" s="13">
+        <f t="shared" ref="D4:D10" si="1">E19</f>
+        <v>9.6812804408460416</v>
+      </c>
+      <c r="E4" s="13">
+        <f t="shared" ref="E4:E10" si="2">H19</f>
+        <v>10.20172775501298</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="13">
+        <f t="shared" si="0"/>
+        <v>130174.7515586768</v>
+      </c>
+      <c r="D5" s="13">
+        <f t="shared" si="1"/>
+        <v>94.892898436960735</v>
+      </c>
+      <c r="E5" s="13">
+        <f t="shared" si="2"/>
+        <v>100.7710073442213</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D6" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E6" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="13">
+        <f t="shared" si="0"/>
+        <v>6.5565514492500014</v>
+      </c>
+      <c r="D7" s="13">
+        <f t="shared" si="1"/>
+        <v>0.86619144197884357</v>
+      </c>
+      <c r="E7" s="13">
+        <f t="shared" si="2"/>
+        <v>0.86494869959436882</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="13">
+        <f t="shared" si="0"/>
+        <v>1363</v>
+      </c>
+      <c r="D8" s="13">
+        <f t="shared" si="1"/>
+        <v>2.3991141732283459</v>
+      </c>
+      <c r="E8" s="13">
+        <f t="shared" si="2"/>
+        <v>2.4171331899999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="13">
+        <f t="shared" si="0"/>
+        <v>5668</v>
+      </c>
+      <c r="D9" s="13">
+        <f t="shared" si="1"/>
+        <v>6.088816312733635</v>
+      </c>
+      <c r="E9" s="13">
+        <f t="shared" si="2"/>
+        <v>6.1963116119999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="13">
+        <f t="shared" si="0"/>
+        <v>10713002</v>
+      </c>
+      <c r="D10" s="13">
+        <f t="shared" si="1"/>
+        <v>6656.7508251809431</v>
+      </c>
+      <c r="E10" s="13">
+        <f t="shared" si="2"/>
+        <v>6656.7508251809431</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18">
+        <v>55496</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18">
+        <v>52485</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18">
+        <v>49927</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19">
+        <v>10532.358433133521</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19">
+        <v>9.6812804408460416</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H19">
+        <v>10.20172775501298</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20">
+        <v>130174.7515586768</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20">
+        <v>94.892898436960735</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H20">
+        <v>100.7710073442213</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22">
+        <v>6.5565514492500014</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22">
+        <v>0.86619144197884357</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H22">
+        <v>0.86494869959436882</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23">
+        <v>1363</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23">
+        <v>2.3991141732283459</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H23">
+        <v>2.4171331899999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24">
+        <v>5668</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24">
+        <v>6.088816312733635</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H24">
+        <v>6.1963116119999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25">
+        <v>10713002</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25">
+        <v>6656.7508251809431</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H25">
+        <v>6656.7508251809431</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>42</v>
       </c>
@@ -8427,11 +9618,8 @@
       <c r="D1" t="s">
         <v>43</v>
       </c>
-      <c r="E1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>A15</f>
         <v>count</v>
@@ -8444,16 +9632,12 @@
         <f>E15</f>
         <v>52477</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="4">
         <f>H15</f>
-        <v>49763</v>
-      </c>
-      <c r="E2">
-        <f>K15</f>
         <v>49732</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f t="shared" ref="A3:B9" si="0">A16</f>
         <v>mean</v>
@@ -8466,16 +9650,12 @@
         <f t="shared" ref="C3:C9" si="1">E16</f>
         <v>17.22436074964482</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="4">
         <f t="shared" ref="D3:D9" si="2">H16</f>
-        <v>23.235513735104298</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E9" si="3">K16</f>
         <v>23.241758425158771</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>std</v>
@@ -8488,16 +9668,12 @@
         <f t="shared" si="1"/>
         <v>205.11247607787021</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="4">
         <f t="shared" si="2"/>
-        <v>407.71964374523287</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="3"/>
         <v>407.84633734050658</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>min</v>
@@ -8510,16 +9686,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E5">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>25%</v>
@@ -8532,16 +9704,12 @@
         <f t="shared" si="1"/>
         <v>4.7351491483285999</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="4">
         <f t="shared" si="2"/>
         <v>4.6100000000000003</v>
       </c>
-      <c r="E6">
-        <f t="shared" si="3"/>
-        <v>4.6100000000000003</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>50%</v>
@@ -8554,16 +9722,12 @@
         <f t="shared" si="1"/>
         <v>10.804398947999999</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="4">
         <f t="shared" si="2"/>
         <v>10.63</v>
       </c>
-      <c r="E7">
-        <f t="shared" si="3"/>
-        <v>10.63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>75%</v>
@@ -8576,16 +9740,12 @@
         <f t="shared" si="1"/>
         <v>18.543628287722768</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="4">
         <f t="shared" si="2"/>
-        <v>18.600000000000001</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="3"/>
         <v>18.62</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>max</v>
@@ -8598,24 +9758,23 @@
         <f t="shared" si="1"/>
         <v>31782.813369919659</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="4">
         <f t="shared" si="2"/>
         <v>38155.39</v>
       </c>
-      <c r="E9">
-        <f t="shared" si="3"/>
-        <v>38155.39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
       <c r="D13" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>34</v>
       </c>
@@ -8625,11 +9784,8 @@
       <c r="H14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K14" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
@@ -8646,84 +9802,231 @@
         <v>26</v>
       </c>
       <c r="H15">
-        <v>49763</v>
+        <v>49732</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16">
+        <v>22.494156482753311</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16">
+        <v>17.22436074964482</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16">
+        <v>23.241758425158771</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17">
+        <v>387.10086169451358</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17">
+        <v>205.11247607787021</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H17">
+        <v>407.84633734050658</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19">
+        <v>4.7</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19">
+        <v>4.7351491483285999</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19">
+        <v>4.6100000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20">
+        <v>10.67</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20">
+        <v>10.804398947999999</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H20">
+        <v>10.63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21">
+        <v>18.66</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21">
+        <v>18.543628287722768</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H21">
+        <v>18.62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22">
+        <v>38155.39</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22">
+        <v>31782.813369919659</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H22">
+        <v>38155.39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{399845A7-C827-4756-BAAD-0176948427C8}">
+  <dimension ref="F14:K27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14:K22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="14" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="G14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15">
+        <v>55496</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>26</v>
       </c>
       <c r="K15">
-        <v>49732</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+        <v>52485</v>
+      </c>
+    </row>
+    <row r="16" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B16">
-        <v>22.494156482753311</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16">
-        <v>17.22436074964482</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>27</v>
+      <c r="G16">
+        <v>808.27993008505121</v>
       </c>
       <c r="H16">
-        <v>23.235513735104298</v>
+        <f>G16/60</f>
+        <v>13.471332168084187</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K16">
-        <v>23.241758425158771</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+        <v>18.665536820043819</v>
+      </c>
+    </row>
+    <row r="17" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B17">
-        <v>387.10086169451358</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17">
-        <v>205.11247607787021</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>28</v>
+      <c r="G17">
+        <v>1698.399567912207</v>
       </c>
       <c r="H17">
-        <v>407.71964374523287</v>
+        <f t="shared" ref="H17:H22" si="0">G17/60</f>
+        <v>28.306659465203449</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>28</v>
       </c>
       <c r="K17">
-        <v>407.84633734050658</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+        <v>50.576568422141293</v>
+      </c>
+    </row>
+    <row r="18" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B18">
+      <c r="G18">
         <v>0</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="H18">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J18" s="1" t="s">
@@ -8733,108 +10036,81 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F19" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B19">
-        <v>4.7</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19">
-        <v>4.7351491483285999</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>30</v>
+      <c r="G19">
+        <v>15</v>
       </c>
       <c r="H19">
-        <v>4.6100000000000003</v>
+        <f t="shared" si="0"/>
+        <v>0.25</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>30</v>
       </c>
       <c r="K19">
-        <v>4.6100000000000003</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F20" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B20">
-        <v>10.67</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20">
-        <v>10.804398947999999</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>31</v>
+      <c r="G20">
+        <v>472</v>
       </c>
       <c r="H20">
-        <v>10.63</v>
+        <f t="shared" si="0"/>
+        <v>7.8666666666666663</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>31</v>
       </c>
       <c r="K20">
-        <v>10.63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F21" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B21">
-        <v>18.66</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21">
-        <v>18.543628287722768</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>32</v>
+      <c r="G21">
+        <v>1051</v>
       </c>
       <c r="H21">
-        <v>18.600000000000001</v>
+        <f t="shared" si="0"/>
+        <v>17.516666666666666</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>32</v>
       </c>
       <c r="K21">
-        <v>18.62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F22" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B22">
-        <v>38155.39</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E22">
-        <v>31782.813369919659</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>33</v>
+      <c r="G22">
+        <v>108050</v>
       </c>
       <c r="H22">
-        <v>38155.39</v>
+        <f t="shared" si="0"/>
+        <v>1800.8333333333333</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>33</v>
       </c>
       <c r="K22">
-        <v>38155.39</v>
+        <v>2709</v>
+      </c>
+    </row>
+    <row r="27" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="I27" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>